<commit_message>
aktualizace pro PDF export (včetně)
</commit_message>
<xml_diff>
--- a/K odevzdání/Use Case - Požadavky.xlsx
+++ b/K odevzdání/Use Case - Požadavky.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505"/>
@@ -370,7 +370,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -383,9 +383,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kancelář">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,7 +423,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kancelář">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -495,7 +495,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kancelář">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -669,6 +669,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
@@ -1161,7 +1164,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>